<commit_message>
added template version: 0.2
</commit_message>
<xml_diff>
--- a/Documents/Work_Plan.xlsx
+++ b/Documents/Work_Plan.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -18,9 +18,80 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>Week 1</t>
+  </si>
+  <si>
+    <t>Week 2</t>
+  </si>
+  <si>
+    <t>Week 3</t>
+  </si>
+  <si>
+    <t>Week 4</t>
+  </si>
+  <si>
+    <t>Week 5</t>
+  </si>
+  <si>
+    <t>Week 6</t>
+  </si>
+  <si>
+    <t>Week 7</t>
+  </si>
+  <si>
+    <t>Week 8</t>
+  </si>
+  <si>
+    <t>Week 9</t>
+  </si>
+  <si>
+    <t>Week 10</t>
+  </si>
+  <si>
+    <t>Week 11</t>
+  </si>
+  <si>
+    <t>Week 12</t>
+  </si>
+  <si>
+    <t>Updated Project Work Plan / LR /SRS/ SDO</t>
+  </si>
+  <si>
+    <t>Test Plan Document</t>
+  </si>
+  <si>
+    <t>Midterm Interactive-DEMO</t>
+  </si>
+  <si>
+    <t>Final Product 1st Release</t>
+  </si>
+  <si>
+    <t>User Manual</t>
+  </si>
+  <si>
+    <t>Project Report / Test Result / Project Tracking Form</t>
+  </si>
+  <si>
+    <t>Project Poster</t>
+  </si>
+  <si>
+    <t>Updated Project Webpage</t>
+  </si>
+  <si>
+    <t>DEMO Video</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,13 +99,40 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -46,13 +144,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="%20 - Vurgu1" xfId="2" builtinId="30"/>
+    <cellStyle name="İyi" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -323,7 +428,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -331,12 +436,165 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <cols>
+    <col min="1" max="1" width="45.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="3"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="M3" s="3"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="M4" s="3"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="M5" s="3"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="M6" s="3"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="M7" s="3"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="M8" s="3"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="M9" s="3"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="M10" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Edited on dates and determined the work plan
</commit_message>
<xml_diff>
--- a/Documents/Work_Plan.xlsx
+++ b/Documents/Work_Plan.xlsx
@@ -1,26 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\407\project\ceng-407-408-2022-2023-Surroundings-Detection-System-for-Visually-Impaired-People-GenEye\Documents\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C383A2A-D570-48F6-B1CC-134E8C09FC07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-3852" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="28125" windowHeight="13080"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -96,20 +85,32 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="162"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
       <charset val="162"/>
       <scheme val="minor"/>
     </font>
@@ -117,20 +118,148 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="162"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="162"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -139,23 +268,210 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -163,32 +479,341 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="58" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="58" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="23"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="23" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="25" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="25" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="25"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -237,7 +862,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -272,7 +897,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -446,249 +1071,259 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="B1:N12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.44140625" customWidth="1"/>
-    <col min="2" max="2" width="36.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="10" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.43809523809524" customWidth="1"/>
+    <col min="2" max="2" width="39.1428571428571" customWidth="1"/>
+    <col min="3" max="3" width="12.4285714285714" customWidth="1"/>
+    <col min="4" max="4" width="12.2857142857143" customWidth="1"/>
+    <col min="5" max="5" width="11.8571428571429" customWidth="1"/>
+    <col min="6" max="6" width="11.2857142857143" customWidth="1"/>
+    <col min="7" max="7" width="11.7142857142857" customWidth="1"/>
+    <col min="8" max="8" width="11.4285714285714" customWidth="1"/>
+    <col min="9" max="9" width="11.7142857142857" customWidth="1"/>
+    <col min="10" max="10" width="11.5714285714286" customWidth="1"/>
+    <col min="11" max="11" width="11.7142857142857" customWidth="1"/>
+    <col min="12" max="12" width="11.2857142857143" customWidth="1"/>
+    <col min="13" max="13" width="11.7142857142857" customWidth="1"/>
+    <col min="14" max="14" width="11.2857142857143" customWidth="1"/>
+    <col min="17" max="17" width="15" customWidth="1"/>
+    <col min="18" max="18" width="14.2857142857143" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="C1" s="4">
+    <row r="1" spans="3:14">
+      <c r="C1" s="1">
         <v>44844</v>
       </c>
-      <c r="D1" s="4">
+      <c r="D1" s="2">
         <v>44851</v>
       </c>
-      <c r="E1" s="4">
+      <c r="E1" s="2">
         <v>44858</v>
       </c>
-      <c r="F1" s="4">
+      <c r="F1" s="2">
         <v>44865</v>
       </c>
-      <c r="G1" s="4">
+      <c r="G1" s="2">
         <v>44872</v>
       </c>
-      <c r="H1" s="4">
+      <c r="H1" s="2">
         <v>44879</v>
       </c>
-      <c r="I1" s="4">
+      <c r="I1" s="2">
         <v>44886</v>
       </c>
-      <c r="J1" s="4">
+      <c r="J1" s="2">
         <v>44893</v>
       </c>
-      <c r="K1" s="4">
+      <c r="K1" s="2">
         <v>44900</v>
       </c>
-      <c r="L1" s="4">
+      <c r="L1" s="2">
         <v>44907</v>
       </c>
-      <c r="M1" s="4">
+      <c r="M1" s="2">
         <v>44914</v>
       </c>
-      <c r="N1" s="4">
+      <c r="N1" s="2">
         <v>44921</v>
       </c>
     </row>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="C2" s="4">
+    <row r="2" spans="3:14">
+      <c r="C2" s="1">
         <v>44848</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="2">
         <v>44855</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="2">
         <v>44862</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="2">
         <v>44869</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="2">
         <v>44876</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="2">
         <v>44883</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="2">
         <v>44890</v>
       </c>
-      <c r="J2" s="4">
+      <c r="J2" s="2">
         <v>44897</v>
       </c>
-      <c r="K2" s="4">
+      <c r="K2" s="2">
         <v>44904</v>
       </c>
-      <c r="L2" s="4">
+      <c r="L2" s="2">
         <v>44911</v>
       </c>
-      <c r="M2" s="4">
+      <c r="M2" s="2">
         <v>44918</v>
       </c>
-      <c r="N2" s="4">
+      <c r="N2" s="2">
         <v>44925</v>
       </c>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B3" s="1" t="s">
+    <row r="3" spans="2:14">
+      <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="L3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="M3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="N3" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B4" s="3" t="s">
+    <row r="4" spans="2:14">
+      <c r="B4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="N4" s="2"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="7"/>
+      <c r="F4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="N4" s="8"/>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B5" s="3" t="s">
+    <row r="5" spans="2:14">
+      <c r="B5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="N5" s="2"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="N5" s="8"/>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B6" s="3" t="s">
+    <row r="6" spans="2:14">
+      <c r="B6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="N6" s="2"/>
+      <c r="D6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="N6" s="8"/>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B7" s="3" t="s">
+    <row r="7" spans="2:14">
+      <c r="B7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="N7" s="2"/>
+      <c r="D7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="N7" s="8"/>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="3" t="s">
+    <row r="8" spans="2:14">
+      <c r="B8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="N8" s="2"/>
+      <c r="D8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="N8" s="8"/>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B9" s="3" t="s">
+    <row r="9" spans="2:14">
+      <c r="B9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="N9" s="2"/>
+      <c r="D9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="N9" s="8"/>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B10" s="3" t="s">
+    <row r="10" spans="2:14">
+      <c r="B10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="N10" s="2"/>
+      <c r="D10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="N10" s="8"/>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B11" s="3" t="s">
+    <row r="11" spans="2:14">
+      <c r="B11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="N11" s="2"/>
+      <c r="D11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="N11" s="8"/>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B12" s="3" t="s">
+    <row r="12" spans="2:14">
+      <c r="B12" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="N12" s="2"/>
+      <c r="D12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="N12" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>